<commit_message>
some fake data to test household_id
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_HHID.xlsx
+++ b/data-raw/FAKE_DATA_HHID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872B2803-83F6-7E49-AA50-5A07E967B915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53420017-DA7E-6E47-A29B-9E11E86386A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="660" windowWidth="22800" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="960" yWindow="660" windowWidth="24640" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>NNSS</t>
   </si>
@@ -123,6 +123,75 @@
   </si>
   <si>
     <t>Ben</t>
+  </si>
+  <si>
+    <t>Bamberger</t>
+  </si>
+  <si>
+    <t>Barth</t>
+  </si>
+  <si>
+    <t>Barth-Bechtel</t>
+  </si>
+  <si>
+    <t>Berg-Becker</t>
+  </si>
+  <si>
+    <t>Bickel</t>
+  </si>
+  <si>
+    <t>Caduff</t>
+  </si>
+  <si>
+    <t>Bloom</t>
+  </si>
+  <si>
+    <t>Bischoff</t>
+  </si>
+  <si>
+    <t>Bayer</t>
+  </si>
+  <si>
+    <t>Babsi</t>
+  </si>
+  <si>
+    <t>Banu</t>
+  </si>
+  <si>
+    <t>Bailee</t>
+  </si>
+  <si>
+    <t>Barbora</t>
+  </si>
+  <si>
+    <t>Basilia</t>
+  </si>
+  <si>
+    <t>Beate</t>
+  </si>
+  <si>
+    <t>Bella</t>
+  </si>
+  <si>
+    <t>Bellina</t>
+  </si>
+  <si>
+    <t>Belmira</t>
+  </si>
+  <si>
+    <t>Belma</t>
+  </si>
+  <si>
+    <t>Beatrix</t>
+  </si>
+  <si>
+    <t>Bea</t>
+  </si>
+  <si>
+    <t>Batul</t>
+  </si>
+  <si>
+    <t>Becky</t>
   </si>
 </sst>
 </file>
@@ -173,14 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,292 +611,586 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>7560000000010</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>4019</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>7560000000011</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>8069</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>7560000000012</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>12116</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>2</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>7560000000013</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>16166</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5">
-        <v>3</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>7560000000014</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>20214</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="5">
-        <v>3</v>
-      </c>
-      <c r="I6" s="5">
-        <v>3</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>7560000000015</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>24264</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5">
-        <v>3</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5">
-        <v>3</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7560000000016</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>28313</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="5">
-        <v>3</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="5">
-        <v>3</v>
-      </c>
-      <c r="I8" s="5">
-        <v>3</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="H8" s="4">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>7560000000016</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>7560000000017</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>32363</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="5">
-        <v>3</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="5">
-        <v>3</v>
-      </c>
-      <c r="I9" s="5">
-        <v>3</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>7560000000016</v>
-      </c>
-      <c r="B10" s="4" t="s">
+        <v>7560000000018</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>36412</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="5">
-        <v>3</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="5">
-        <v>3</v>
-      </c>
-      <c r="I10" s="5">
-        <v>3</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="4">
+        <v>3</v>
+      </c>
+      <c r="J10" s="4">
         <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>7560000000019</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>7560000000020</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
+        <v>4</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>7560000000021</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <v>4</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>7560000000022</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>4</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>7560000000023</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>4</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>7560000000024</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>4</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>7560000000025</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>4</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>7560000000026</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>4</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>7560000000027</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3</v>
+      </c>
+      <c r="H19" s="4">
+        <v>4</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>7560000000028</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3</v>
+      </c>
+      <c r="H20" s="4">
+        <v>4</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>7560000000029</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="4">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>4</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>7560000000030</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>7560000000031</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>7560000000032</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>